<commit_message>
Added Jupyter notebooks for Windischleuba 2024
</commit_message>
<xml_diff>
--- a/PraktikumPhysik/LineareRegression.xlsx
+++ b/PraktikumPhysik/LineareRegression.xlsx
@@ -5,17 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertsmith/Documents/GitHub/ConferenceExamples/PraktikumPhysik/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertsmith/Documents/GitHub.nosync/ConferenceExamples/PraktikumPhysik/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1C47E9-EE76-6840-87DC-1DCA0B82A76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7122D07A-2A5D-0545-95B1-DB73A5F87685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8280" yWindow="1840" windowWidth="35200" windowHeight="25480" activeTab="1" xr2:uid="{D544D1D7-07A1-1A47-B933-60B877826460}"/>
+    <workbookView xWindow="5940" yWindow="1660" windowWidth="33600" windowHeight="20500" xr2:uid="{D544D1D7-07A1-1A47-B933-60B877826460}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet2!$B$5:$B$14</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet2!$C$5:$C$14</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Extinktion</t>
   </si>
@@ -113,16 +118,29 @@
     <t>N</t>
   </si>
   <si>
-    <t>u(b)</t>
+    <t>y(Gerechnet)</t>
+  </si>
+  <si>
+    <t>(y-y_ger)^2</t>
+  </si>
+  <si>
+    <t>https://github.com/alsinmr/ConferenceExamples/tree/master/PraktikumPhysik</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="40"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -149,11 +167,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -171,7 +190,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -503,7 +522,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -541,7 +560,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1661279007"/>
@@ -620,7 +639,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -658,7 +677,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1629306799"/>
@@ -710,7 +729,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -747,7 +766,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -761,7 +780,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -798,7 +817,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -852,6 +871,50 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$3:$B$12</c:f>
@@ -1020,7 +1083,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1058,7 +1121,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1661279007"/>
@@ -1137,7 +1200,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1175,7 +1238,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1629306799"/>
@@ -1227,7 +1290,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1264,12 +1327,548 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.40376377952755904"/>
+          <c:y val="4.6296296296296294E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-D5C0-1343-A4B4-33806B903E67}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$5:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$5:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D5C0-1343-A4B4-33806B903E67}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$5:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$I$5:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.16000000000000081</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39933333333333398</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63866666666666716</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87800000000000034</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1173333333333335</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3566666666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5959999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.835333333333333</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0746666666666664</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.3139999999999992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D5C0-1343-A4B4-33806B903E67}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="417313904"/>
+        <c:axId val="416851344"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="417313904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="416851344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="416851344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="417313904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1316,6 +1915,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2387,6 +3026,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2402,8 +3557,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>172528</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="Textfeld 6">
@@ -3036,7 +4191,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="Textfeld 6">
@@ -3349,8 +4504,8 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>14375</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="Textfeld 5">
@@ -3596,7 +4751,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="Textfeld 5">
@@ -3903,15 +5058,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>783771</xdr:colOff>
+      <xdr:colOff>757034</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>402771</xdr:colOff>
+      <xdr:colOff>376034</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>188614</xdr:rowOff>
+      <xdr:rowOff>188613</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -3928,8 +5083,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5600700" y="3868058"/>
-              <a:ext cx="4572000" cy="910699"/>
+              <a:off x="5583034" y="4086726"/>
+              <a:ext cx="4592053" cy="914519"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4550,8 +5705,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5600700" y="3868058"/>
-              <a:ext cx="4572000" cy="910699"/>
+              <a:off x="5583034" y="4086726"/>
+              <a:ext cx="4592053" cy="914519"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4719,8 +5874,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>16257</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 9">
@@ -5287,7 +6442,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 9">
@@ -5459,16 +6614,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>821871</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>90715</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4309</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>106590</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>440871</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>55458</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>448809</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>193135</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -5485,8 +6640,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5638800" y="3283858"/>
-              <a:ext cx="4572000" cy="763029"/>
+              <a:off x="2337934" y="5678715"/>
+              <a:ext cx="4572000" cy="912045"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5636,7 +6791,7 @@
                         <m:subHide m:val="on"/>
                         <m:supHide m:val="on"/>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" i="1">
+                          <a:rPr lang="en-US" sz="2200" i="1">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -5650,7 +6805,7 @@
                         <m:sSubSup>
                           <m:sSubSupPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" i="1">
+                              <a:rPr lang="en-US" sz="2200" i="1">
                                 <a:solidFill>
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
@@ -5663,7 +6818,7 @@
                               <m:rPr>
                                 <m:sty m:val="p"/>
                               </m:rPr>
-                              <a:rPr lang="en-US" i="0">
+                              <a:rPr lang="en-US" sz="2200" i="0">
                                 <a:solidFill>
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
@@ -5674,7 +6829,7 @@
                           </m:e>
                           <m:sub>
                             <m:r>
-                              <a:rPr lang="en-US" i="1">
+                              <a:rPr lang="en-US" sz="2200" i="1">
                                 <a:solidFill>
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
@@ -5685,7 +6840,7 @@
                           </m:sub>
                           <m:sup>
                             <m:r>
-                              <a:rPr lang="en-US" i="0">
+                              <a:rPr lang="en-US" sz="2200" i="0">
                                 <a:solidFill>
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
@@ -5698,7 +6853,7 @@
                       </m:e>
                     </m:nary>
                     <m:r>
-                      <a:rPr lang="en-US" i="0">
+                      <a:rPr lang="en-US" sz="2200" i="0">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
                       <m:t>=</m:t>
@@ -5709,7 +6864,7 @@
                         <m:subHide m:val="on"/>
                         <m:supHide m:val="on"/>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" i="1">
+                          <a:rPr lang="en-US" sz="2200" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -5720,7 +6875,7 @@
                         <m:sSubSup>
                           <m:sSubSupPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" i="1">
+                              <a:rPr lang="en-US" sz="2200" i="1">
                                 <a:solidFill>
                                   <a:srgbClr val="836967"/>
                                 </a:solidFill>
@@ -5730,7 +6885,7 @@
                           </m:sSubSupPr>
                           <m:e>
                             <m:r>
-                              <a:rPr lang="en-US" i="1">
+                              <a:rPr lang="en-US" sz="2200" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>𝑦</m:t>
@@ -5738,7 +6893,7 @@
                           </m:e>
                           <m:sub>
                             <m:r>
-                              <a:rPr lang="en-US" i="1">
+                              <a:rPr lang="en-US" sz="2200" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>𝑖</m:t>
@@ -5746,7 +6901,7 @@
                           </m:sub>
                           <m:sup>
                             <m:r>
-                              <a:rPr lang="en-US" i="0">
+                              <a:rPr lang="en-US" sz="2200" i="0">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>2</m:t>
@@ -5756,7 +6911,7 @@
                       </m:e>
                     </m:nary>
                     <m:r>
-                      <a:rPr lang="en-US" i="0">
+                      <a:rPr lang="en-US" sz="2200" i="0">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
                       <m:t>−</m:t>
@@ -5765,7 +6920,7 @@
                       <m:barPr>
                         <m:pos m:val="top"/>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" i="1">
+                          <a:rPr lang="en-US" sz="2200" i="1">
                             <a:solidFill>
                               <a:srgbClr val="836967"/>
                             </a:solidFill>
@@ -5775,7 +6930,7 @@
                       </m:barPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="en-US" i="1">
+                          <a:rPr lang="en-US" sz="2200" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                           <m:t>𝑏</m:t>
@@ -5788,7 +6943,7 @@
                         <m:subHide m:val="on"/>
                         <m:supHide m:val="on"/>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" i="1">
+                          <a:rPr lang="en-US" sz="2200" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -5799,7 +6954,7 @@
                         <m:sSub>
                           <m:sSubPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" i="1">
+                              <a:rPr lang="en-US" sz="2200" i="1">
                                 <a:solidFill>
                                   <a:srgbClr val="836967"/>
                                 </a:solidFill>
@@ -5809,7 +6964,7 @@
                           </m:sSubPr>
                           <m:e>
                             <m:r>
-                              <a:rPr lang="en-US" i="1">
+                              <a:rPr lang="en-US" sz="2200" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>𝑦</m:t>
@@ -5817,7 +6972,7 @@
                           </m:e>
                           <m:sub>
                             <m:r>
-                              <a:rPr lang="en-US" i="1">
+                              <a:rPr lang="en-US" sz="2200" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>𝑖</m:t>
@@ -5827,7 +6982,7 @@
                         <m:sSub>
                           <m:sSubPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" i="1">
+                              <a:rPr lang="en-US" sz="2200" i="1">
                                 <a:solidFill>
                                   <a:srgbClr val="836967"/>
                                 </a:solidFill>
@@ -5837,7 +6992,7 @@
                           </m:sSubPr>
                           <m:e>
                             <m:r>
-                              <a:rPr lang="en-US" i="1">
+                              <a:rPr lang="en-US" sz="2200" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>𝑥</m:t>
@@ -5845,7 +7000,7 @@
                           </m:e>
                           <m:sub>
                             <m:r>
-                              <a:rPr lang="en-US" i="1">
+                              <a:rPr lang="en-US" sz="2200" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>𝑖</m:t>
@@ -5855,7 +7010,7 @@
                       </m:e>
                     </m:nary>
                     <m:r>
-                      <a:rPr lang="en-US" i="0">
+                      <a:rPr lang="en-US" sz="2200" i="0">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
                       <m:t>−</m:t>
@@ -5864,7 +7019,7 @@
                       <m:barPr>
                         <m:pos m:val="top"/>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" i="1">
+                          <a:rPr lang="en-US" sz="2200" i="1">
                             <a:solidFill>
                               <a:srgbClr val="836967"/>
                             </a:solidFill>
@@ -5874,7 +7029,7 @@
                       </m:barPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="en-US" i="1">
+                          <a:rPr lang="en-US" sz="2200" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                           <m:t>𝑎</m:t>
@@ -5887,7 +7042,7 @@
                         <m:subHide m:val="on"/>
                         <m:supHide m:val="on"/>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" i="1">
+                          <a:rPr lang="en-US" sz="2200" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -5898,7 +7053,7 @@
                         <m:sSub>
                           <m:sSubPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" i="1">
+                              <a:rPr lang="en-US" sz="2200" i="1">
                                 <a:solidFill>
                                   <a:srgbClr val="836967"/>
                                 </a:solidFill>
@@ -5908,7 +7063,7 @@
                           </m:sSubPr>
                           <m:e>
                             <m:r>
-                              <a:rPr lang="en-US" i="1">
+                              <a:rPr lang="en-US" sz="2200" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>𝑦</m:t>
@@ -5916,7 +7071,7 @@
                           </m:e>
                           <m:sub>
                             <m:r>
-                              <a:rPr lang="en-US" i="1">
+                              <a:rPr lang="en-US" sz="2200" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>𝑖</m:t>
@@ -5928,7 +7083,7 @@
                   </m:oMath>
                 </m:oMathPara>
               </a14:m>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-US" sz="2200"/>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -5947,8 +7102,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5638800" y="3283858"/>
-              <a:ext cx="4572000" cy="763029"/>
+              <a:off x="2337934" y="5678715"/>
+              <a:ext cx="4572000" cy="912045"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6087,7 +7242,7 @@
             <a:p>
               <a:pPr/>
               <a:r>
-                <a:rPr lang="en-US" i="0">
+                <a:rPr lang="en-US" sz="2200" i="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -6096,13 +7251,13 @@
                 <a:t>∑▒ν_𝑖^2 </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" i="0">
+                <a:rPr lang="en-US" sz="2200" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>=∑▒𝑦</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" i="0">
+                <a:rPr lang="en-US" sz="2200" i="0">
                   <a:solidFill>
                     <a:srgbClr val="836967"/>
                   </a:solidFill>
@@ -6111,13 +7266,13 @@
                 <a:t>_</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" i="0">
+                <a:rPr lang="en-US" sz="2200" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>𝑖^2 −</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" i="0">
+                <a:rPr lang="en-US" sz="2200" i="0">
                   <a:solidFill>
                     <a:srgbClr val="836967"/>
                   </a:solidFill>
@@ -6126,13 +7281,13 @@
                 <a:t>¯</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" i="0">
+                <a:rPr lang="en-US" sz="2200" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>𝑏 ∑▒〖𝑦</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" i="0">
+                <a:rPr lang="en-US" sz="2200" i="0">
                   <a:solidFill>
                     <a:srgbClr val="836967"/>
                   </a:solidFill>
@@ -6141,13 +7296,13 @@
                 <a:t>_</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" i="0">
+                <a:rPr lang="en-US" sz="2200" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>𝑖</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" i="0">
+                <a:rPr lang="en-US" sz="2200" i="0">
                   <a:solidFill>
                     <a:srgbClr val="836967"/>
                   </a:solidFill>
@@ -6156,13 +7311,13 @@
                 <a:t> </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" i="0">
+                <a:rPr lang="en-US" sz="2200" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>𝑥</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" i="0">
+                <a:rPr lang="en-US" sz="2200" i="0">
                   <a:solidFill>
                     <a:srgbClr val="836967"/>
                   </a:solidFill>
@@ -6171,13 +7326,13 @@
                 <a:t>_</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" i="0">
+                <a:rPr lang="en-US" sz="2200" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>𝑖 〗−</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" i="0">
+                <a:rPr lang="en-US" sz="2200" i="0">
                   <a:solidFill>
                     <a:srgbClr val="836967"/>
                   </a:solidFill>
@@ -6186,13 +7341,13 @@
                 <a:t>¯</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" i="0">
+                <a:rPr lang="en-US" sz="2200" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>𝑎 ∑▒𝑦</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" i="0">
+                <a:rPr lang="en-US" sz="2200" i="0">
                   <a:solidFill>
                     <a:srgbClr val="836967"/>
                   </a:solidFill>
@@ -6201,12 +7356,12 @@
                 <a:t>_</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" i="0">
+                <a:rPr lang="en-US" sz="2200" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>𝑖 </a:t>
               </a:r>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-US" sz="2200"/>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -6221,16 +7376,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>37420</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>344656</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>130344</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>333829</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>85215</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>479594</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>138461</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -6247,8 +7402,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="5395233"/>
-              <a:ext cx="4451407" cy="444670"/>
+              <a:off x="8633077" y="731923"/>
+              <a:ext cx="4279149" cy="810222"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6393,14 +7548,14 @@
                   </m:oMathParaPr>
                   <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                     <m:r>
-                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                      <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                       </a:rPr>
                       <m:t>𝑏</m:t>
                     </m:r>
                     <m:r>
-                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                      <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                       </a:rPr>
@@ -6409,7 +7564,7 @@
                     <m:f>
                       <m:fPr>
                         <m:ctrlPr>
-                          <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                          <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                           </a:rPr>
@@ -6420,7 +7575,7 @@
                           <m:naryPr>
                             <m:chr m:val="∑"/>
                             <m:ctrlPr>
-                              <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                              <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
@@ -6431,14 +7586,14 @@
                               <m:rPr>
                                 <m:brk m:alnAt="23"/>
                               </m:rPr>
-                              <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                              <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
                               <m:t>𝑖</m:t>
                             </m:r>
                             <m:r>
-                              <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                              <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
@@ -6447,7 +7602,7 @@
                           </m:sub>
                           <m:sup>
                             <m:r>
-                              <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                              <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
@@ -6458,7 +7613,7 @@
                             <m:d>
                               <m:dPr>
                                 <m:ctrlPr>
-                                  <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                                  <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                                     <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                   </a:rPr>
@@ -6468,7 +7623,7 @@
                                 <m:sSub>
                                   <m:sSubPr>
                                     <m:ctrlPr>
-                                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                                      <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                       </a:rPr>
@@ -6476,7 +7631,7 @@
                                   </m:sSubPr>
                                   <m:e>
                                     <m:r>
-                                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                                      <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                       </a:rPr>
@@ -6485,7 +7640,7 @@
                                   </m:e>
                                   <m:sub>
                                     <m:r>
-                                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                                      <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                       </a:rPr>
@@ -6496,7 +7651,7 @@
                                 <m:sSub>
                                   <m:sSubPr>
                                     <m:ctrlPr>
-                                      <a:rPr lang="de-DE" sz="1400" i="1">
+                                      <a:rPr lang="de-DE" sz="2400" i="1">
                                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                       </a:rPr>
@@ -6504,7 +7659,7 @@
                                   </m:sSubPr>
                                   <m:e>
                                     <m:r>
-                                      <a:rPr lang="de-DE" sz="1400" i="1">
+                                      <a:rPr lang="de-DE" sz="2400" i="1">
                                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
@@ -6512,7 +7667,7 @@
                                       <m:t>∙</m:t>
                                     </m:r>
                                     <m:r>
-                                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                                      <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                       </a:rPr>
@@ -6521,7 +7676,7 @@
                                   </m:e>
                                   <m:sub>
                                     <m:r>
-                                      <a:rPr lang="de-DE" sz="1400" i="1">
+                                      <a:rPr lang="de-DE" sz="2400" i="1">
                                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                       </a:rPr>
@@ -6532,7 +7687,7 @@
                               </m:e>
                             </m:d>
                             <m:r>
-                              <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                              <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
@@ -6542,7 +7697,7 @@
                               <m:accPr>
                                 <m:chr m:val="̅"/>
                                 <m:ctrlPr>
-                                  <a:rPr lang="de-DE" sz="1400" i="1">
+                                  <a:rPr lang="de-DE" sz="2400" i="1">
                                     <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                   </a:rPr>
@@ -6550,7 +7705,7 @@
                               </m:accPr>
                               <m:e>
                                 <m:r>
-                                  <a:rPr lang="de-DE" sz="1400" i="1">
+                                  <a:rPr lang="de-DE" sz="2400" i="1">
                                     <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                   </a:rPr>
@@ -6561,7 +7716,7 @@
                           </m:e>
                         </m:nary>
                         <m:r>
-                          <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                          <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
@@ -6572,7 +7727,7 @@
                           <m:naryPr>
                             <m:chr m:val="∑"/>
                             <m:ctrlPr>
-                              <a:rPr lang="de-DE" sz="1400" i="1">
+                              <a:rPr lang="de-DE" sz="2400" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
@@ -6583,14 +7738,14 @@
                               <m:rPr>
                                 <m:brk m:alnAt="23"/>
                               </m:rPr>
-                              <a:rPr lang="de-DE" sz="1400" i="1">
+                              <a:rPr lang="de-DE" sz="2400" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
                               <m:t>𝑖</m:t>
                             </m:r>
                             <m:r>
-                              <a:rPr lang="de-DE" sz="1400" i="1">
+                              <a:rPr lang="de-DE" sz="2400" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
@@ -6599,7 +7754,7 @@
                           </m:sub>
                           <m:sup>
                             <m:r>
-                              <a:rPr lang="de-DE" sz="1400" i="1">
+                              <a:rPr lang="de-DE" sz="2400" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
@@ -6610,7 +7765,7 @@
                             <m:sSub>
                               <m:sSubPr>
                                 <m:ctrlPr>
-                                  <a:rPr lang="de-DE" sz="1400" i="1">
+                                  <a:rPr lang="de-DE" sz="2400" i="1">
                                     <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                   </a:rPr>
@@ -6618,7 +7773,7 @@
                               </m:sSubPr>
                               <m:e>
                                 <m:r>
-                                  <a:rPr lang="de-DE" sz="1400" i="1">
+                                  <a:rPr lang="de-DE" sz="2400" i="1">
                                     <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                   </a:rPr>
@@ -6627,7 +7782,7 @@
                               </m:e>
                               <m:sub>
                                 <m:r>
-                                  <a:rPr lang="de-DE" sz="1400" i="1">
+                                  <a:rPr lang="de-DE" sz="2400" i="1">
                                     <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                   </a:rPr>
@@ -6643,7 +7798,7 @@
                           <m:naryPr>
                             <m:chr m:val="∑"/>
                             <m:ctrlPr>
-                              <a:rPr lang="de-DE" sz="1400" i="1">
+                              <a:rPr lang="de-DE" sz="2400" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
@@ -6654,14 +7809,14 @@
                               <m:rPr>
                                 <m:brk m:alnAt="23"/>
                               </m:rPr>
-                              <a:rPr lang="de-DE" sz="1400" i="1">
+                              <a:rPr lang="de-DE" sz="2400" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
                               <m:t>𝑖</m:t>
                             </m:r>
                             <m:r>
-                              <a:rPr lang="de-DE" sz="1400" i="1">
+                              <a:rPr lang="de-DE" sz="2400" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
@@ -6670,7 +7825,7 @@
                           </m:sub>
                           <m:sup>
                             <m:r>
-                              <a:rPr lang="de-DE" sz="1400" i="1">
+                              <a:rPr lang="de-DE" sz="2400" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
@@ -6681,7 +7836,7 @@
                             <m:sSup>
                               <m:sSupPr>
                                 <m:ctrlPr>
-                                  <a:rPr lang="de-DE" sz="1400" i="1">
+                                  <a:rPr lang="de-DE" sz="2400" i="1">
                                     <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                   </a:rPr>
@@ -6691,7 +7846,7 @@
                                 <m:sSub>
                                   <m:sSubPr>
                                     <m:ctrlPr>
-                                      <a:rPr lang="de-DE" sz="1400" i="1">
+                                      <a:rPr lang="de-DE" sz="2400" i="1">
                                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                       </a:rPr>
@@ -6699,7 +7854,7 @@
                                   </m:sSubPr>
                                   <m:e>
                                     <m:r>
-                                      <a:rPr lang="de-DE" sz="1400" i="1">
+                                      <a:rPr lang="de-DE" sz="2400" i="1">
                                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                       </a:rPr>
@@ -6708,7 +7863,7 @@
                                   </m:e>
                                   <m:sub>
                                     <m:r>
-                                      <a:rPr lang="de-DE" sz="1400" i="1">
+                                      <a:rPr lang="de-DE" sz="2400" i="1">
                                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                       </a:rPr>
@@ -6719,7 +7874,7 @@
                               </m:e>
                               <m:sup>
                                 <m:r>
-                                  <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                                  <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                                     <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                   </a:rPr>
@@ -6728,7 +7883,7 @@
                               </m:sup>
                             </m:sSup>
                             <m:r>
-                              <a:rPr lang="de-DE" sz="1400" i="1">
+                              <a:rPr lang="de-DE" sz="2400" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
@@ -6738,7 +7893,7 @@
                               <m:accPr>
                                 <m:chr m:val="̅"/>
                                 <m:ctrlPr>
-                                  <a:rPr lang="de-DE" sz="1400" i="1">
+                                  <a:rPr lang="de-DE" sz="2400" i="1">
                                     <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                   </a:rPr>
@@ -6746,7 +7901,7 @@
                               </m:accPr>
                               <m:e>
                                 <m:r>
-                                  <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                                  <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                                     <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                   </a:rPr>
@@ -6757,7 +7912,7 @@
                           </m:e>
                         </m:nary>
                         <m:r>
-                          <a:rPr lang="de-DE" sz="1400" i="1">
+                          <a:rPr lang="de-DE" sz="2400" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
@@ -6768,7 +7923,7 @@
                           <m:naryPr>
                             <m:chr m:val="∑"/>
                             <m:ctrlPr>
-                              <a:rPr lang="de-DE" sz="1400" i="1">
+                              <a:rPr lang="de-DE" sz="2400" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
@@ -6779,14 +7934,14 @@
                               <m:rPr>
                                 <m:brk m:alnAt="23"/>
                               </m:rPr>
-                              <a:rPr lang="de-DE" sz="1400" i="1">
+                              <a:rPr lang="de-DE" sz="2400" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
                               <m:t>𝑖</m:t>
                             </m:r>
                             <m:r>
-                              <a:rPr lang="de-DE" sz="1400" i="1">
+                              <a:rPr lang="de-DE" sz="2400" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
@@ -6795,7 +7950,7 @@
                           </m:sub>
                           <m:sup>
                             <m:r>
-                              <a:rPr lang="de-DE" sz="1400" i="1">
+                              <a:rPr lang="de-DE" sz="2400" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                               </a:rPr>
@@ -6806,7 +7961,7 @@
                             <m:sSub>
                               <m:sSubPr>
                                 <m:ctrlPr>
-                                  <a:rPr lang="de-DE" sz="1400" i="1">
+                                  <a:rPr lang="de-DE" sz="2400" i="1">
                                     <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                   </a:rPr>
@@ -6814,7 +7969,7 @@
                               </m:sSubPr>
                               <m:e>
                                 <m:r>
-                                  <a:rPr lang="de-DE" sz="1400" i="1">
+                                  <a:rPr lang="de-DE" sz="2400" i="1">
                                     <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                   </a:rPr>
@@ -6823,7 +7978,7 @@
                               </m:e>
                               <m:sub>
                                 <m:r>
-                                  <a:rPr lang="de-DE" sz="1400" i="1">
+                                  <a:rPr lang="de-DE" sz="2400" i="1">
                                     <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                                   </a:rPr>
@@ -6839,7 +7994,7 @@
                       <m:accPr>
                         <m:chr m:val="̅"/>
                         <m:ctrlPr>
-                          <a:rPr lang="de-DE" sz="1400" i="1">
+                          <a:rPr lang="de-DE" sz="2400" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                           </a:rPr>
@@ -6847,7 +8002,7 @@
                       </m:accPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                          <a:rPr lang="de-DE" sz="2400" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                           </a:rPr>
@@ -6858,7 +8013,7 @@
                   </m:oMath>
                 </m:oMathPara>
               </a14:m>
-              <a:endParaRPr lang="en-GB" sz="1400" i="0">
+              <a:endParaRPr lang="en-GB" sz="2400" i="0">
                 <a:latin typeface="+mn-lt"/>
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:endParaRPr>
@@ -6880,8 +8035,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="5395233"/>
-              <a:ext cx="4451407" cy="444670"/>
+              <a:off x="8633077" y="731923"/>
+              <a:ext cx="4279149" cy="810222"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7020,14 +8175,14 @@
             <a:p>
               <a:pPr/>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" b="0" i="0">
+                <a:rPr lang="de-DE" sz="2400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>𝑏=(∑_(𝑖=1)^𝑛▒〖(𝑥_𝑖 〖</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" i="0">
+                <a:rPr lang="de-DE" sz="2400" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
@@ -7035,42 +8190,42 @@
                 <a:t>∙</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" b="0" i="0">
+                <a:rPr lang="de-DE" sz="2400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>𝑦〗_</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" i="0">
+                <a:rPr lang="de-DE" sz="2400" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>𝑖 )</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" b="0" i="0">
+                <a:rPr lang="de-DE" sz="2400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>−</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" i="0">
+                <a:rPr lang="de-DE" sz="2400" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>𝑦 ̅ </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" b="0" i="0">
+                <a:rPr lang="de-DE" sz="2400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>〗</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" b="0" i="0">
+                <a:rPr lang="de-DE" sz="2400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
@@ -7078,63 +8233,63 @@
                 <a:t>∙∑_(</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" i="0">
+                <a:rPr lang="de-DE" sz="2400" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>𝑖=1)^𝑛▒𝑥_𝑖 </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" b="0" i="0">
+                <a:rPr lang="de-DE" sz="2400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>)/(∑_(</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" i="0">
+                <a:rPr lang="de-DE" sz="2400" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>𝑖=1)^𝑛</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" b="0" i="0">
+                <a:rPr lang="de-DE" sz="2400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>▒〖〖</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" i="0">
+                <a:rPr lang="de-DE" sz="2400" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>𝑥_𝑖〗^</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" b="0" i="0">
+                <a:rPr lang="de-DE" sz="2400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>2</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" i="0">
+                <a:rPr lang="de-DE" sz="2400" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>−</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" b="0" i="0">
+                <a:rPr lang="de-DE" sz="2400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>𝑥 ̅ 〗</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" i="0">
+                <a:rPr lang="de-DE" sz="2400" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
@@ -7142,20 +8297,20 @@
                 <a:t>∙∑_(</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" i="0">
+                <a:rPr lang="de-DE" sz="2400" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>𝑖=1)^𝑛▒𝑥_𝑖 </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" b="0" i="0">
+                <a:rPr lang="de-DE" sz="2400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>) 𝑥 ̅</a:t>
               </a:r>
-              <a:endParaRPr lang="en-GB" sz="1400" i="0">
+              <a:endParaRPr lang="en-GB" sz="2400" i="0">
                 <a:latin typeface="+mn-lt"/>
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:endParaRPr>
@@ -7168,16 +8323,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>515938</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>110217</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>201780</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>150322</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>66606</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>119377</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>581290</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>93660</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -7194,8 +8349,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="515938" y="6063342"/>
-              <a:ext cx="2021215" cy="207598"/>
+              <a:off x="8490201" y="1955059"/>
+              <a:ext cx="2037194" cy="344390"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7340,14 +8495,14 @@
                   </m:oMathParaPr>
                   <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                     <m:r>
-                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                      <a:rPr lang="de-DE" sz="2200" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                       </a:rPr>
                       <m:t>𝑎</m:t>
                     </m:r>
                     <m:r>
-                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                      <a:rPr lang="de-DE" sz="2200" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                       </a:rPr>
@@ -7357,7 +8512,7 @@
                       <m:accPr>
                         <m:chr m:val="̅"/>
                         <m:ctrlPr>
-                          <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                          <a:rPr lang="de-DE" sz="2200" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                           </a:rPr>
@@ -7365,7 +8520,7 @@
                       </m:accPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                          <a:rPr lang="de-DE" sz="2200" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                           </a:rPr>
@@ -7374,21 +8529,21 @@
                       </m:e>
                     </m:acc>
                     <m:r>
-                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                      <a:rPr lang="de-DE" sz="2200" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                       </a:rPr>
                       <m:t>−</m:t>
                     </m:r>
                     <m:r>
-                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                      <a:rPr lang="de-DE" sz="2200" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                       </a:rPr>
                       <m:t>𝑏</m:t>
                     </m:r>
                     <m:r>
-                      <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                      <a:rPr lang="de-DE" sz="2200" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
@@ -7399,7 +8554,7 @@
                       <m:accPr>
                         <m:chr m:val="̅"/>
                         <m:ctrlPr>
-                          <a:rPr lang="de-DE" sz="1400" i="1">
+                          <a:rPr lang="de-DE" sz="2200" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                           </a:rPr>
@@ -7407,7 +8562,7 @@
                       </m:accPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="de-DE" sz="1400" b="0" i="1">
+                          <a:rPr lang="de-DE" sz="2200" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                           </a:rPr>
@@ -7418,7 +8573,7 @@
                   </m:oMath>
                 </m:oMathPara>
               </a14:m>
-              <a:endParaRPr lang="en-GB" sz="1400" i="0">
+              <a:endParaRPr lang="en-GB" sz="2200" i="0">
                 <a:latin typeface="+mn-lt"/>
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:endParaRPr>
@@ -7440,8 +8595,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="515938" y="6063342"/>
-              <a:ext cx="2021215" cy="207598"/>
+              <a:off x="8490201" y="1955059"/>
+              <a:ext cx="2037194" cy="344390"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7580,14 +8735,14 @@
             <a:p>
               <a:pPr/>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" b="0" i="0">
+                <a:rPr lang="de-DE" sz="2200" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>𝑎=𝑦 ̅−𝑏</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" b="0" i="0">
+                <a:rPr lang="de-DE" sz="2200" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
@@ -7595,13 +8750,13 @@
                 <a:t>∙</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1400" b="0" i="0">
+                <a:rPr lang="de-DE" sz="2200" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:rPr>
                 <a:t>𝑥 ̅</a:t>
               </a:r>
-              <a:endParaRPr lang="en-GB" sz="1400" i="0">
+              <a:endParaRPr lang="en-GB" sz="2200" i="0">
                 <a:latin typeface="+mn-lt"/>
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:endParaRPr>
@@ -7658,16 +8813,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>54146</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>809792</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>100935</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>107950</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>147282</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>428792</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>194071</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -7684,8 +8839,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5430044" y="5808834"/>
-              <a:ext cx="4560094" cy="886886"/>
+              <a:off x="4954003" y="5114093"/>
+              <a:ext cx="4592052" cy="895241"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -8306,8 +9461,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5430044" y="5808834"/>
-              <a:ext cx="4560094" cy="886886"/>
+              <a:off x="4954003" y="5114093"/>
+              <a:ext cx="4592052" cy="895241"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -8465,15 +9620,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>565547</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>17237</xdr:rowOff>
+      <xdr:colOff>4074</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>3868</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>184547</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>110373</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>451916</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>97004</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -8490,8 +9645,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5506641" y="5176612"/>
-              <a:ext cx="4560094" cy="886886"/>
+              <a:off x="4977127" y="4415447"/>
+              <a:ext cx="4592052" cy="895241"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -9057,8 +10212,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5506641" y="5176612"/>
-              <a:ext cx="4560094" cy="886886"/>
+              <a:off x="4977127" y="4415447"/>
+              <a:ext cx="4592052" cy="895241"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -9216,15 +10371,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>29936</xdr:rowOff>
+      <xdr:colOff>184485</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>83410</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>178603</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>632327</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>31551</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -9241,8 +10396,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5626894" y="4593999"/>
-              <a:ext cx="4560094" cy="743979"/>
+              <a:off x="5157538" y="3893410"/>
+              <a:ext cx="4592052" cy="750246"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -9703,8 +10858,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5626894" y="4593999"/>
-              <a:ext cx="4560094" cy="743979"/>
+              <a:off x="5157538" y="3893410"/>
+              <a:ext cx="4592052" cy="750246"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -9983,8 +11138,8 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>110022</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="Textfeld 5">
@@ -10205,7 +11360,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="Textfeld 5">
@@ -10413,11 +11568,47 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>33421</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>175794</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>461210</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>111626</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Diagramm 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFE69134-B32B-4E6F-8EF1-9A8EDDAEDA3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -10715,8 +11906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A477BA73-DCE7-1A4D-BC5B-E741D85AC4F9}">
   <dimension ref="A2:N21"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10771,7 +11962,7 @@
         <v>4.0000000000000008E-2</v>
       </c>
       <c r="K3">
-        <f>B$21+B$20*B3</f>
+        <f t="shared" ref="K3:K12" si="0">B$21+B$20*B3</f>
         <v>0.16000000000000081</v>
       </c>
       <c r="M3">
@@ -10779,7 +11970,7 @@
         <v>1.5999999999999363E-3</v>
       </c>
       <c r="N3">
-        <f>(C3-C$18)^2</f>
+        <f t="shared" ref="N3:N12" si="1">(C3-C$18)^2</f>
         <v>1.0753690000000002</v>
       </c>
     </row>
@@ -10792,27 +11983,27 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E12" si="0">B4^2</f>
+        <f t="shared" ref="E4:E12" si="2">B4^2</f>
         <v>4.0000000000000008E-2</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F12" si="1">B4*C4</f>
+        <f t="shared" ref="F4:F12" si="3">B4*C4</f>
         <v>0.11000000000000001</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G12" si="2">C4^2</f>
+        <f t="shared" ref="G4:G12" si="4">C4^2</f>
         <v>0.30250000000000005</v>
       </c>
       <c r="K4">
-        <f>B$21+B$20*B4</f>
+        <f t="shared" si="0"/>
         <v>0.39933333333333398</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M12" si="3">(K4-C4)^2</f>
+        <f t="shared" ref="M4:M12" si="5">(K4-C4)^2</f>
         <v>2.2700444444444263E-2</v>
       </c>
       <c r="N4">
-        <f>(C4-C$18)^2</f>
+        <f t="shared" si="1"/>
         <v>0.47196900000000008</v>
       </c>
     </row>
@@ -10825,27 +12016,27 @@
         <v>0.6</v>
       </c>
       <c r="E5">
+        <f t="shared" si="2"/>
+        <v>0.09</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="3"/>
+        <v>0.18</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="4"/>
+        <v>0.36</v>
+      </c>
+      <c r="K5">
         <f t="shared" si="0"/>
-        <v>0.09</v>
-      </c>
-      <c r="F5">
+        <v>0.63866666666666716</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="5"/>
+        <v>1.495111111111151E-3</v>
+      </c>
+      <c r="N5">
         <f t="shared" si="1"/>
-        <v>0.18</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="2"/>
-        <v>0.36</v>
-      </c>
-      <c r="K5">
-        <f>B$21+B$20*B5</f>
-        <v>0.63866666666666716</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="3"/>
-        <v>1.495111111111151E-3</v>
-      </c>
-      <c r="N5">
-        <f>(C5-C$18)^2</f>
         <v>0.40576900000000016</v>
       </c>
     </row>
@@ -10858,27 +12049,27 @@
         <v>0.82</v>
       </c>
       <c r="E6">
+        <f t="shared" si="2"/>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="3"/>
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="4"/>
+        <v>0.67239999999999989</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="0"/>
-        <v>0.16000000000000003</v>
-      </c>
-      <c r="F6">
+        <v>0.87800000000000034</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="5"/>
+        <v>3.3640000000000445E-3</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="1"/>
-        <v>0.32800000000000001</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="2"/>
-        <v>0.67239999999999989</v>
-      </c>
-      <c r="K6">
-        <f>B$21+B$20*B6</f>
-        <v>0.87800000000000034</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="3"/>
-        <v>3.3640000000000445E-3</v>
-      </c>
-      <c r="N6">
-        <f>(C6-C$18)^2</f>
         <v>0.17388900000000013</v>
       </c>
     </row>
@@ -10891,27 +12082,27 @@
         <v>0.9</v>
       </c>
       <c r="E7">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="3"/>
+        <v>0.45</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="4"/>
+        <v>0.81</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="F7">
+        <v>1.1173333333333335</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="5"/>
+        <v>4.7233777777777847E-2</v>
+      </c>
+      <c r="N7">
         <f t="shared" si="1"/>
-        <v>0.45</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="2"/>
-        <v>0.81</v>
-      </c>
-      <c r="K7">
-        <f>B$21+B$20*B7</f>
-        <v>1.1173333333333335</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="3"/>
-        <v>4.7233777777777847E-2</v>
-      </c>
-      <c r="N7">
-        <f>(C7-C$18)^2</f>
         <v>0.11356900000000006</v>
       </c>
     </row>
@@ -10924,27 +12115,27 @@
         <v>1.4</v>
       </c>
       <c r="E8">
+        <f t="shared" si="2"/>
+        <v>0.36</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="3"/>
+        <v>0.84</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="4"/>
+        <v>1.9599999999999997</v>
+      </c>
+      <c r="K8">
         <f t="shared" si="0"/>
-        <v>0.36</v>
-      </c>
-      <c r="F8">
+        <v>1.3566666666666667</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="5"/>
+        <v>1.8777777777777684E-3</v>
+      </c>
+      <c r="N8">
         <f t="shared" si="1"/>
-        <v>0.84</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="2"/>
-        <v>1.9599999999999997</v>
-      </c>
-      <c r="K8">
-        <f>B$21+B$20*B8</f>
-        <v>1.3566666666666667</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="3"/>
-        <v>1.8777777777777684E-3</v>
-      </c>
-      <c r="N8">
-        <f>(C8-C$18)^2</f>
         <v>2.656899999999994E-2</v>
       </c>
     </row>
@@ -10957,27 +12148,27 @@
         <v>1.5</v>
       </c>
       <c r="E9">
+        <f t="shared" si="2"/>
+        <v>0.48999999999999994</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="3"/>
+        <v>1.0499999999999998</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="4"/>
+        <v>2.25</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="0"/>
-        <v>0.48999999999999994</v>
-      </c>
-      <c r="F9">
+        <v>1.5959999999999999</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="5"/>
+        <v>9.2159999999999742E-3</v>
+      </c>
+      <c r="N9">
         <f t="shared" si="1"/>
-        <v>1.0499999999999998</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="2"/>
-        <v>2.25</v>
-      </c>
-      <c r="K9">
-        <f>B$21+B$20*B9</f>
-        <v>1.5959999999999999</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="3"/>
-        <v>9.2159999999999742E-3</v>
-      </c>
-      <c r="N9">
-        <f>(C9-C$18)^2</f>
         <v>6.9168999999999953E-2</v>
       </c>
     </row>
@@ -10990,27 +12181,27 @@
         <v>1.9</v>
       </c>
       <c r="E10">
+        <f t="shared" si="2"/>
+        <v>0.64000000000000012</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="3"/>
+        <v>1.52</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="4"/>
+        <v>3.61</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="0"/>
-        <v>0.64000000000000012</v>
-      </c>
-      <c r="F10">
+        <v>1.835333333333333</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="5"/>
+        <v>4.1817777777778042E-3</v>
+      </c>
+      <c r="N10">
         <f t="shared" si="1"/>
-        <v>1.52</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="2"/>
-        <v>3.61</v>
-      </c>
-      <c r="K10">
-        <f>B$21+B$20*B10</f>
-        <v>1.835333333333333</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="3"/>
-        <v>4.1817777777778042E-3</v>
-      </c>
-      <c r="N10">
-        <f>(C10-C$18)^2</f>
         <v>0.43956899999999977</v>
       </c>
     </row>
@@ -11023,27 +12214,27 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E11">
+        <f t="shared" si="2"/>
+        <v>0.81</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="3"/>
+        <v>1.9800000000000002</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="4"/>
+        <v>4.8400000000000007</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="0"/>
-        <v>0.81</v>
-      </c>
-      <c r="F11">
+        <v>2.0746666666666664</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="5"/>
+        <v>1.5708444444444546E-2</v>
+      </c>
+      <c r="N11">
         <f t="shared" si="1"/>
-        <v>1.9800000000000002</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="2"/>
-        <v>4.8400000000000007</v>
-      </c>
-      <c r="K11">
-        <f>B$21+B$20*B11</f>
-        <v>2.0746666666666664</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="3"/>
-        <v>1.5708444444444546E-2</v>
-      </c>
-      <c r="N11">
-        <f>(C11-C$18)^2</f>
         <v>0.92736900000000011</v>
       </c>
     </row>
@@ -11056,27 +12247,27 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="3"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="4"/>
+        <v>5.2899999999999991</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F12">
+        <v>2.3139999999999992</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="5"/>
+        <v>1.959999999999817E-4</v>
+      </c>
+      <c r="N12">
         <f t="shared" si="1"/>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="2"/>
-        <v>5.2899999999999991</v>
-      </c>
-      <c r="K12">
-        <f>B$21+B$20*B12</f>
-        <v>2.3139999999999992</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="3"/>
-        <v>1.959999999999817E-4</v>
-      </c>
-      <c r="N12">
-        <f>(C12-C$18)^2</f>
         <v>1.1299689999999993</v>
       </c>
     </row>
@@ -11210,16 +12401,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5909B351-99F3-B046-8021-327EC9596807}">
-  <dimension ref="A3:G21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78097117-B244-E742-B7CA-C6EC0C95B86C}">
+  <dimension ref="I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="9:9" ht="52" x14ac:dyDescent="0.6">
+      <c r="I28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5909B351-99F3-B046-8021-327EC9596807}">
+  <dimension ref="A3:J20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>21</v>
       </c>
@@ -11227,7 +12438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>22</v>
       </c>
@@ -11235,16 +12446,22 @@
         <v>23</v>
       </c>
       <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
       </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>0.1</v>
       </c>
@@ -11253,19 +12470,27 @@
         <v>0.2</v>
       </c>
       <c r="E5">
+        <f>B5*C5</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="F5">
         <f>B5^2</f>
         <v>1.0000000000000002E-2</v>
-      </c>
-      <c r="F5">
-        <f>B5*C5</f>
-        <v>2.0000000000000004E-2</v>
       </c>
       <c r="G5">
         <f>C5^2</f>
         <v>4.0000000000000008E-2</v>
       </c>
+      <c r="I5">
+        <f>$B$20+B$19*B5</f>
+        <v>0.16000000000000081</v>
+      </c>
+      <c r="J5">
+        <f>(I5-C5)^2</f>
+        <v>1.5999999999999363E-3</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>0.2</v>
       </c>
@@ -11274,19 +12499,27 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E14" si="0">B6^2</f>
+        <f>B6*C6</f>
+        <v>0.11000000000000001</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F14" si="0">B6^2</f>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="F6">
-        <f t="shared" ref="F6:F14" si="1">B6*C6</f>
-        <v>0.11000000000000001</v>
-      </c>
       <c r="G6">
-        <f t="shared" ref="G6:G14" si="2">C6^2</f>
+        <f t="shared" ref="G6:G14" si="1">C6^2</f>
         <v>0.30250000000000005</v>
       </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I14" si="2">$B$20+B$19*B6</f>
+        <v>0.39933333333333398</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J14" si="3">(I6-C6)^2</f>
+        <v>2.2700444444444263E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>0.3</v>
       </c>
@@ -11295,19 +12528,27 @@
         <v>0.6</v>
       </c>
       <c r="E7">
+        <f t="shared" ref="E6:E14" si="4">B7*C7</f>
+        <v>0.18</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <f t="shared" si="1"/>
-        <v>0.18</v>
-      </c>
-      <c r="G7">
+        <v>0.36</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="2"/>
-        <v>0.36</v>
+        <v>0.63866666666666716</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>1.495111111111151E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>0.4</v>
       </c>
@@ -11316,19 +12557,27 @@
         <v>0.82</v>
       </c>
       <c r="E8">
+        <f t="shared" si="4"/>
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="0"/>
         <v>0.16000000000000003</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <f t="shared" si="1"/>
-        <v>0.32800000000000001</v>
-      </c>
-      <c r="G8">
+        <v>0.67239999999999989</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="2"/>
-        <v>0.67239999999999989</v>
+        <v>0.87800000000000034</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>3.3640000000000445E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>0.5</v>
       </c>
@@ -11337,19 +12586,27 @@
         <v>0.9</v>
       </c>
       <c r="E9">
+        <f t="shared" si="4"/>
+        <v>0.45</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <f t="shared" si="1"/>
-        <v>0.45</v>
-      </c>
-      <c r="G9">
+        <v>0.81</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="2"/>
-        <v>0.81</v>
+        <v>1.1173333333333335</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>4.7233777777777847E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>0.6</v>
       </c>
@@ -11358,19 +12615,27 @@
         <v>1.4</v>
       </c>
       <c r="E10">
+        <f t="shared" si="4"/>
+        <v>0.84</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <f t="shared" si="1"/>
-        <v>0.84</v>
-      </c>
-      <c r="G10">
+        <v>1.9599999999999997</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="2"/>
-        <v>1.9599999999999997</v>
+        <v>1.3566666666666667</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>1.8777777777777684E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>0.7</v>
       </c>
@@ -11379,19 +12644,27 @@
         <v>1.5</v>
       </c>
       <c r="E11">
+        <f t="shared" si="4"/>
+        <v>1.0499999999999998</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="0"/>
         <v>0.48999999999999994</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <f t="shared" si="1"/>
-        <v>1.0499999999999998</v>
-      </c>
-      <c r="G11">
+        <v>2.25</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="2"/>
-        <v>2.25</v>
+        <v>1.5959999999999999</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>9.2159999999999742E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>0.8</v>
       </c>
@@ -11400,19 +12673,27 @@
         <v>1.9</v>
       </c>
       <c r="E12">
+        <f t="shared" si="4"/>
+        <v>1.52</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="0"/>
         <v>0.64000000000000012</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <f t="shared" si="1"/>
-        <v>1.52</v>
-      </c>
-      <c r="G12">
+        <v>3.61</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="2"/>
-        <v>3.61</v>
+        <v>1.835333333333333</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>4.1817777777778042E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>0.9</v>
       </c>
@@ -11421,19 +12702,27 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E13">
+        <f t="shared" si="4"/>
+        <v>1.9800000000000002</v>
+      </c>
+      <c r="F13">
         <f t="shared" si="0"/>
         <v>0.81</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <f t="shared" si="1"/>
-        <v>1.9800000000000002</v>
-      </c>
-      <c r="G13">
+        <v>4.8400000000000007</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="2"/>
-        <v>4.8400000000000007</v>
+        <v>2.0746666666666664</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>1.5708444444444546E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>1</v>
       </c>
@@ -11442,95 +12731,88 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E14">
+        <f t="shared" si="4"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F14">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <f t="shared" si="1"/>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="G14">
+        <v>5.2899999999999991</v>
+      </c>
+      <c r="I14">
         <f t="shared" si="2"/>
-        <v>5.2899999999999991</v>
+        <v>2.3139999999999992</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>1.959999999999817E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B16">
+      <c r="B15">
         <f>COUNTA(B5:B14)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B17">
+      <c r="B16">
         <f>SUM(B5:B14)</f>
         <v>5.5</v>
       </c>
-      <c r="C17">
+      <c r="C16">
         <f>SUM(C5:C14)</f>
         <v>12.370000000000001</v>
       </c>
-      <c r="E17">
+      <c r="E16">
         <f>SUM(E5:E14)</f>
+        <v>8.7779999999999987</v>
+      </c>
+      <c r="F16">
+        <f>SUM(F5:F14)</f>
         <v>3.85</v>
       </c>
-      <c r="F17">
-        <f>SUM(F5:F14)</f>
-        <v>8.7779999999999987</v>
-      </c>
-      <c r="G17">
+      <c r="G16">
         <f>SUM(G5:G14)</f>
         <v>20.134899999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B18">
-        <f>B17/$B16</f>
+      <c r="B17">
+        <f>B16/B15</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="C18">
-        <f t="shared" ref="C18:G18" si="3">C17/$B16</f>
+      <c r="C17">
+        <f>AVERAGE(C5:C14)</f>
         <v>1.2370000000000001</v>
       </c>
-      <c r="E18">
-        <f t="shared" si="3"/>
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="3"/>
-        <v>0.87779999999999991</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="3"/>
-        <v>2.01349</v>
-      </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <f>(E16-C17*B16)/(F16-B17*B16)</f>
+        <v>2.3933333333333318</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B20">
-        <f>(F17-C18*B17)/(E17-B18*B17)</f>
-        <v>2.3933333333333318</v>
-      </c>
-      <c r="D20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21">
-        <f>C18-B20*B18</f>
+        <f>C17-B19*B17</f>
         <v>-7.9333333333332368E-2</v>
       </c>
     </row>

</xml_diff>